<commit_message>
Updated to Week 6
</commit_message>
<xml_diff>
--- a/BachelorSeason21.xlsx
+++ b/BachelorSeason21.xlsx
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O2" t="s">
         <v>116</v>
@@ -925,7 +925,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q2">
-        <v>8.0000000000000004E-4</v>
+        <v>0.01</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O4" t="s">
         <v>120</v>
@@ -1093,7 +1093,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q5">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>0.10393851452</v>
       </c>
       <c r="Q7">
-        <v>0.22840984071500001</v>
+        <v>0.162678571429</v>
       </c>
       <c r="R7">
         <v>0.25</v>
@@ -1258,13 +1258,13 @@
         <v>124</v>
       </c>
       <c r="P8">
-        <v>0.10393851452</v>
+        <v>0.177623054172</v>
       </c>
       <c r="Q8">
-        <v>0.13849264069299999</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O9" t="s">
         <v>125</v>
@@ -1317,7 +1317,7 @@
         <v>0.177623054172</v>
       </c>
       <c r="Q9">
-        <v>0.12760904761899999</v>
+        <v>0.125</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1370,10 +1370,10 @@
         <v>126</v>
       </c>
       <c r="P10">
-        <v>0.10393851452</v>
+        <v>0.177623054172</v>
       </c>
       <c r="Q10">
-        <v>4.0969999999999999E-2</v>
+        <v>0.42</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1485,7 +1485,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q12">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q14">
-        <v>8.0000000000000004E-4</v>
+        <v>0.01</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1653,7 +1653,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q15">
-        <v>8.0000000000000004E-4</v>
+        <v>0.01</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O16" t="s">
         <v>129</v>
@@ -1709,7 +1709,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q16">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1812,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O18" t="s">
         <v>148</v>
@@ -1821,7 +1821,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q18">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O19" t="s">
         <v>130</v>
@@ -1930,10 +1930,10 @@
         <v>131</v>
       </c>
       <c r="P20">
-        <v>0.10393851452</v>
+        <v>0.177623054172</v>
       </c>
       <c r="Q20">
-        <v>0.18693248196199999</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q22">
-        <v>4.0000000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q24">
-        <v>8.2400000000000001E-2</v>
+        <v>0.06</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -2210,10 +2210,10 @@
         <v>144</v>
       </c>
       <c r="P25">
-        <v>5.9173802578599999E-2</v>
+        <v>0.13285834223000001</v>
       </c>
       <c r="Q25">
-        <v>2.2612380952400001E-2</v>
+        <v>0.21</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2266,13 +2266,13 @@
         <v>134</v>
       </c>
       <c r="P26">
-        <v>0.10393851452</v>
+        <v>0.177623054172</v>
       </c>
       <c r="Q26">
-        <v>0.22840984071500001</v>
+        <v>0.01</v>
       </c>
       <c r="R26">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O27" t="s">
         <v>135</v>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O29" t="s">
         <v>136</v>
@@ -2437,7 +2437,7 @@
         <v>2.23632283267E-3</v>
       </c>
       <c r="Q29">
-        <v>2.3599999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0.10393851452</v>
       </c>
       <c r="Q30">
-        <v>8.5660079365100006E-2</v>
+        <v>7.45238095238E-2</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O31" t="s">
         <v>137</v>

</xml_diff>